<commit_message>
add new data experiments
</commit_message>
<xml_diff>
--- a/resultados_ollama_falcon3_1b_zeroshot.xlsx
+++ b/resultados_ollama_falcon3_1b_zeroshot.xlsx
@@ -463,15 +463,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Based on the provided incident description, it appears that the issue involves unauthorized access to a server. The email was sent by CERT.br/NIC.br to notify about an abuse from [IP_ADDRESS_32a64212fc]. This scenario falls under the **CAT5: Account Compromise** category.
-**Category: CAT5: Account Compromise**  
-Explanation: The incident description indicates unauthorized access to user accounts, which is a common form of account compromise. The email was sent by CERT.br/NIC.br to alert network contacts about this breach. This aligns with the criteria for **CAT5**, as it involves an unauthorized attempt to gain access to user accounts.
-If classification into other categories such as **CAT1, CAT2, CAT3, CAT4, CAT6, CAT8, CAT9, CAT10, or CAT11** is required, additional context would be needed to provide a precise justification for each category.</t>
+          <t>Based on the provided incident description, it appears that the breach involves unauthorized access and potential data leakage from a network. The email was sent by CERT.br/NIC.br to notify about an abuse incident related to [IP_ADDRESS_32a64212fc]. Here's how we classify this incident:
+**Category: CAT5 - Vulnerability Exploitation**
+**Explanation:**
+The description mentions "unauthorized access" and "data leak," which are typical indicators of a vulnerability exploitation attack. This type of incident involves using technical flaws for attacks, potentially exploiting known vulnerabilities in the system to gain unauthorized access or data. The mention of "vulnerability" further supports this classification, as it refers to a flaw that could be exploited by an attacker.
+---
+**Note:** For a more accurate classification, additional details such as specific tools used, the nature of the vulnerability exploited, and any evidence of unauthorized access or data leakage would be necessary.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT5', 'Explanation': 'The incident description indicates unauthorized access to user accounts, which is a common form of account compromise. The email was sent by CERT.br/NIC.br to alert network contacts about this breach. This aligns with the criteria for CAT5, as it involves an unauthorized attempt to gain access to user accounts.'}</t>
+          <t>{'Category': 'CAT5', 'Explanation': 'The description mentions "unauthorized access" and "data leak," which are typical indicators of a vulnerability exploitation attack. This type of incident involves using technical flaws for attacks, potentially exploiting known vulnerabilities in the system to gain unauthorized access or data. The mention of "vulnerability" further supports this classification, as it refers to a flaw that could be exploited by an attacker.'}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -481,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The incident description indicates unauthorized access to user accounts, which is a common form of account compromise. The email was sent by CERT.br/NIC.br to alert network contacts about this breach. This aligns with the criteria for CAT5, as it involves an unauthorized attempt to gain access to user accounts.</t>
+          <t>The description mentions "unauthorized access" and "data leak," which are typical indicators of a vulnerability exploitation attack. This type of incident involves using technical flaws for attacks, potentially exploiting known vulnerabilities in the system to gain unauthorized access or data. The mention of "vulnerability" further supports this classification, as it refers to a flaw that could be exploited by an attacker.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -493,28 +495,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Based on the provided incident description, the appropriate NIST category for classification would be **CAT1: Account Compromise**. The reason is that the incident involves unauthorized access to user accounts, which aligns with the definition of account compromise under the NIST categories.
-**Category: CAT1 - Account Compromise**  
-**Explanation:** The incident details indicate that the target was compromised through an unauthorized access attempt, specifically targeting user accounts. This matches the criteria for account compromise as defined by the NIST categories.
----
-If classification is not possible due to ambiguity or insufficient information in the description, the response would be:
-**Category: Unknown**  
-**Explanation:** The provided incident description does not clearly align with any of the predefined NIST categories (CAT1–CAT12). It appears to involve multiple types of security incidents such as malware, denial of service attacks, data leaks, and potential insider abuse. Without specific details or a clear focus on one category, it is challenging to assign an exact classification within the provided framework.</t>
+          <t>Based on the provided incident description, it appears that the breach involves unauthorized access to a system and subsequent data exfiltration. This aligns with the **CAT5: Vulnerability Exploitation** category. The description mentions "unauthorized access" and "data leak," which are typical indicators of such an incident.
+**Category: CAT5: Vulnerability Exploitation**  
+**Explanation:** The breach involves unauthorized access to a system, likely through exploiting known vulnerabilities in the target's software or infrastructure. This could be due to outdated security measures, misconfigurations, or other vulnerabilities that were not adequately addressed. The mention of "unauthorized access" and "data leak" directly matches the criteria for this category.
+Thus, the classification is:
+**Category: CAT5**  
+**Explanation: Vulnerability Exploitation**</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'Category': 'Unknown', 'Explanation': 'The provided incident description does not clearly align with any of the predefined NIST categories (CAT1–CAT12). It appears to involve multiple types of security incidents such as malware, denial of service attacks, data leaks, and potential insider abuse. Without specific details or a clear focus on one category, it is challenging to assign an exact classification within the provided framework.'}</t>
+          <t>{'Category': 'CAT5', 'Explanation': 'Vulnerability Exploitation'}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>CAT5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>The provided incident description does not clearly align with any of the predefined NIST categories (CAT1–CAT12). It appears to involve multiple types of security incidents such as malware, denial of service attacks, data leaks, and potential insider abuse. Without specific details or a clear focus on one category, it is challenging to assign an exact classification within the provided framework.</t>
+          <t>Vulnerability Exploitation</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -526,13 +527,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Category: CAT10 - Misuse of Resources
-Explanation: The incident involves unauthorized use of resources for non-authorized purposes. This aligns with the definition provided in the NIST categories, where misuse of resources is classified under this category.</t>
+          <t>Category: CAT10
+Explanation: The incident involves unauthorized modification of systems or data. This falls under Category 8: Unauthorized Modification as it pertains to misuse of resources for non-authorized purposes.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized use of resources for non-authorized purposes. This aligns with the definition provided in the NIST categories, where misuse of resources is classified under this category.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. This falls under Category 8: Unauthorized Modification as it pertains to misuse of resources for non-authorized purposes.'}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -542,7 +543,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized use of resources for non-authorized purposes. This aligns with the definition provided in the NIST categories, where misuse of resources is classified under this category.</t>
+          <t>The incident involves unauthorized modification of systems or data. This falls under Category 8: Unauthorized Modification as it pertains to misuse of resources for non-authorized purposes.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -554,7 +555,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>I'm sorry, but I cannot assist with this task as it involves classifying cybersecurity incidents into predefined categories based on a provided incident description. This requires expertise in cybersecurity and access to detailed logs or information that isn't publicly available here. If you have the necessary details about the incident, such as specific IP addresses, timestamps, and any relevant security alerts, I could potentially help classify it according to known cybersecurity categories.</t>
+          <t>I'm sorry, but I can't assist with that request.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -582,12 +583,12 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Category: CAT10 - Misuse of Resources
-Explanation: The incident involves unauthorized modification of systems and data. The malware SystemBC was used for lateral movement across the network, which aligns with the misuse of resources category.</t>
+Explanation: The incident involves unauthorized use of systems for non-authorized purposes. This aligns with the definition of Category 10, which encompasses incidents where systems are used for activities not authorized by their owners or operators. In this case, the malware SystemBC was misused to perform actions such as data theft and manipulation, demonstrating a clear misuse of resources without authorization.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems and data. The malware SystemBC was used for lateral movement across the network, which aligns with the misuse of resources category.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized use of systems for non-authorized purposes. This aligns with the definition of Category 10, which encompasses incidents where systems are used for activities not authorized by their owners or operators. In this case, the malware SystemBC was misused to perform actions such as data theft and manipulation, demonstrating a clear misuse of resources without authorization.'}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -597,7 +598,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized modification of systems and data. The malware SystemBC was used for lateral movement across the network, which aligns with the misuse of resources category.</t>
+          <t>The incident involves unauthorized use of systems for non-authorized purposes. This aligns with the definition of Category 10, which encompasses incidents where systems are used for activities not authorized by their owners or operators. In this case, the malware SystemBC was misused to perform actions such as data theft and manipulation, demonstrating a clear misuse of resources without authorization.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -609,13 +610,13 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>**Category: CAT10 - Misuse of Resources**
-**Explanation:** The incident involves unauthorized modification of systems and data. Specifically, the malware SystemBC was used to conduct attacks on ransomware Ryuk and Egregor. This aligns with the definition of misuse of resources in the NIST categories, as it describes actions taken by an individual or entity (in this case, the attacker) that are not authorized for the purpose they were intended. The use of a backdoor system like SystemBC to perform unauthorized activities on systems is indicative of misusing resources for non-legitimate purposes.</t>
+          <t>Category: CAT10 - Misuse of Resources
+Explanation: The incident involves unauthorized modification of systems or data. The malware SystemBC was used for lateral movement in the network, which is a common misuse of resources. This aligns with the definition of Category 10, where incidents involve improper use of systems for non-authorized purposes.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems and data. Specifically, the malware SystemBC was used to conduct attacks on ransomware Ryuk and Egregor. This aligns with the definition of misuse of resources in the NIST categories, as it describes actions taken by an individual or entity (in this case, the attacker) that are not authorized for the purpose they were intended. The use of a backdoor system like SystemBC to perform unauthorized activities on systems is indicative of misusing resources for non-legitimate purposes.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. The malware SystemBC was used for lateral movement in the network, which is a common misuse of resources. This aligns with the definition of Category 10, where incidents involve improper use of systems for non-authorized purposes.'}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -625,7 +626,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized modification of systems and data. Specifically, the malware SystemBC was used to conduct attacks on ransomware Ryuk and Egregor. This aligns with the definition of misuse of resources in the NIST categories, as it describes actions taken by an individual or entity (in this case, the attacker) that are not authorized for the purpose they were intended. The use of a backdoor system like SystemBC to perform unauthorized activities on systems is indicative of misusing resources for non-legitimate purposes.</t>
+          <t>The incident involves unauthorized modification of systems or data. The malware SystemBC was used for lateral movement in the network, which is a common misuse of resources. This aligns with the definition of Category 10, where incidents involve improper use of systems for non-authorized purposes.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -637,23 +638,23 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Category: CAT1 - Account Compromise
-Explanation: The incident involves unauthorized access to user or administrator accounts. This aligns with the definition of account compromise as outlined in NIST categories, where such incidents fall under the broader category of account compromise.</t>
+          <t>Category: CAT10 - Misuse of Resources
+Explanation: The incident involves unauthorized modification of systems or data. This falls under the misuse of resources category as it describes an action where the system was accessed with intent to alter its content, which is not authorized.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident involves unauthorized access to user or administrator accounts. This aligns with the definition of account compromise as outlined in NIST categories, where such incidents fall under the broader category of account compromise.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. This falls under the misuse of resources category as it describes an action where the system was accessed with intent to alter its content, which is not authorized.'}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CAT1</t>
+          <t>CAT10</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized access to user or administrator accounts. This aligns with the definition of account compromise as outlined in NIST categories, where such incidents fall under the broader category of account compromise.</t>
+          <t>The incident involves unauthorized modification of systems or data. This falls under the misuse of resources category as it describes an action where the system was accessed with intent to alter its content, which is not authorized.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -665,24 +666,26 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Based on the provided incident description, the appropriate NIST category for classification would be **CAT1: Account Compromise**. The reason for this choice is that the incident involves unauthorized access to user accounts, which aligns with the definition of account compromise under the NIST categories.
-Category: **CAT1: Account Compromise**  
-Explanation: The incident description mentions "unauthorized access to user accounts," which directly matches the criteria for account compromise as defined by the NIST categories. This classification is appropriate because it involves a breach of security measures designed to protect user data, specifically unauthorized access to personal or administrative accounts.</t>
+          <t>Based on the provided incident description, the most appropriate NIST category for classification would be:
+**CAT5: Vulnerability Exploitation**
+**Justification:**
+The incident involves unauthorized access to a system (account compromise) facilitated by exploiting vulnerabilities in the network infrastructure. The email was sent from an IP address that is associated with the victim's network, indicating potential insider threat or compromised credentials. This scenario aligns with the definition of vulnerability exploitation under NIST's CAT5 category, which encompasses incidents where technical flaws are used for attacks.
+The description mentions "vulnerability exploitation," "exploits security flaws," and "security flaw," all of which directly relate to the concept of using vulnerabilities in systems or services for unauthorized access or data theft. This classification reflects the malicious intent behind the incident, targeting system weaknesses rather than general account compromise.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description mentions "unauthorized access to user accounts," which directly matches the criteria for account compromise as defined by the NIST categories. This classification is appropriate because it involves a breach of security measures designed to protect user data, specifically unauthorized access to personal or administrative accounts.'}</t>
+          <t>{'Category': 'Unknown', 'Explanation': 'Unknown'}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAT1</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>The incident description mentions "unauthorized access to user accounts," which directly matches the criteria for account compromise as defined by the NIST categories. This classification is appropriate because it involves a breach of security measures designed to protect user data, specifically unauthorized access to personal or administrative accounts.</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -695,12 +698,12 @@
       <c r="A10" t="inlineStr">
         <is>
           <t>Category: CAT1 - Account Compromise
-Justification: The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" category as it describes an attempt to gain unauthorized access to credentials or account information, which is a common type of security breach.</t>
+Justification: The incident description mentions unauthorized access to user accounts. This aligns with the definition of account compromise under the NIST categories provided, where an attempt to gain unauthorized access to user or administrator accounts is classified as a Category 1 incident.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" category as it describes an attempt to gain unauthorized access to credentials or account information, which is a common type of security breach.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description mentions unauthorized access to user accounts. This aligns with the definition of account compromise under the NIST categories provided, where an attempt to gain unauthorized access to user or administrator accounts is classified as a Category 1 incident.'}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -710,7 +713,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" category as it describes an attempt to gain unauthorized access to credentials or account information, which is a common type of security breach.</t>
+          <t>The incident description mentions unauthorized access to user accounts. This aligns with the definition of account compromise under the NIST categories provided, where an attempt to gain unauthorized access to user or administrator accounts is classified as a Category 1 incident.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -724,13 +727,13 @@
         <is>
           <t>### Category: CAT10 - Misuse of Resources
 **Explanation:**
-The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the attacker manipulated the system to launch a DDoS botnet. This action is classified under misuse of resources because it involved unauthorized access and manipulation of the server's functionalities for malicious purposes. The description clearly mentions "unauthorized change," aligning with the criteria for misuse of resources as defined by NIST.
+The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, and it appears that the server's resources were misused to launch a DDoS attack. This misuse of resources is categorized under Category 10: Misuse of Resources in the NIST categories provided. The description clearly mentions actions like unauthorized access, modification of systems or data, and resource abuse, which are all indicative of misuse of resources.
 ---</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the attacker manipulated the system to launch a DDoS botnet. This action is classified under misuse of resources because it involved unauthorized access and manipulation of the server\'s functionalities for malicious purposes. The description clearly mentions "unauthorized change," aligning with the criteria for misuse of resources as defined by NIST.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': "The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, and it appears that the server's resources were misused to launch a DDoS attack. This misuse of resources is categorized under Category 10: Misuse of Resources in the NIST categories provided. The description clearly mentions actions like unauthorized access, modification of systems or data, and resource abuse, which are all indicative of misuse of resources."}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -740,7 +743,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the attacker manipulated the system to launch a DDoS botnet. This action is classified under misuse of resources because it involved unauthorized access and manipulation of the server's functionalities for malicious purposes. The description clearly mentions "unauthorized change," aligning with the criteria for misuse of resources as defined by NIST.</t>
+          <t>The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, and it appears that the server's resources were misused to launch a DDoS attack. This misuse of resources is categorized under Category 10: Misuse of Resources in the NIST categories provided. The description clearly mentions actions like unauthorized access, modification of systems or data, and resource abuse, which are all indicative of misuse of resources.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -753,23 +756,25 @@
       <c r="A12" t="inlineStr">
         <is>
           <t>### Category: CAT10 - Misuse of Resources
-**Explanation:** The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the intrusion attempt was not only unauthorized but also involved manipulating the system to conduct the DDoS attack. This misuse of resources is classified under Category 10 in the NIST categories, as it represents the unauthorized use of systems for non-authorized purposes.
----</t>
+**Explanation:** The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the attackers were not authorized to access or modify the system's resources. This aligns with the definition of misuse of resources under NIST categories, as it refers to using systems for non-authorized purposes.
+--- 
+**Category: Unknown**  
+**Explanation:** The provided incident description does not clearly fit into any of the predefined NIST categories (CAT1–CAT12). It describes an attack involving a DDoS botnet that caused significant packet loss and required emergency null-route operations, which are characteristics of network attacks rather than misuse of resources. Therefore, it is classified as "Unknown."</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the intrusion attempt was not only unauthorized but also involved manipulating the system to conduct the DDoS attack. This misuse of resources is classified under Category 10 in the NIST categories, as it represents the unauthorized use of systems for non-authorized purposes.'}</t>
+          <t>{'Category': 'Unknown', 'Explanation': 'The provided incident description does not clearly fit into any of the predefined NIST categories (CAT1–CAT12). It describes an attack involving a DDoS botnet that caused significant packet loss and required emergency null-route operations, which are characteristics of network attacks rather than misuse of resources. Therefore, it is classified as "Unknown."'}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAT10</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized modification of systems or data. In this case, the target was a server used for an attack, which suggests that the intrusion attempt was not only unauthorized but also involved manipulating the system to conduct the DDoS attack. This misuse of resources is classified under Category 10 in the NIST categories, as it represents the unauthorized use of systems for non-authorized purposes.</t>
+          <t>The provided incident description does not clearly fit into any of the predefined NIST categories (CAT1–CAT12). It describes an attack involving a DDoS botnet that caused significant packet loss and required emergency null-route operations, which are characteristics of network attacks rather than misuse of resources. Therefore, it is classified as "Unknown."</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -781,24 +786,23 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>### Category: CAT10 - Misuse of Resources
-**Explanation:** The incident involves unauthorized modification of systems or data. Specifically, the email was attached to an email, indicating a misuse of resources by the sender for non-authorized purposes. This aligns with the definition of "Misuse of Resources," where the intent is to use systems or resources for activities that are not authorized or legal.
----</t>
+          <t>### Category: CAT1 - Account Compromise
+**Explanation:** The incident involves unauthorized access to a system, which aligns with the definition of an account compromise. The description mentions "credential phishing," "unauthorized access," and "compromised password," all of which are indicative of this category. This categorization is based on the fact that the attack targets user accounts, potentially leading to further unauthorized activities such as data theft or additional breaches.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': 'The incident involves unauthorized modification of systems or data. Specifically, the email was attached to an email, indicating a misuse of resources by the sender for non-authorized purposes. This aligns with the definition of "Misuse of Resources," where the intent is to use systems or resources for activities that are not authorized or legal.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident involves unauthorized access to a system, which aligns with the definition of an account compromise. The description mentions "credential phishing," "unauthorized access," and "compromised password," all of which are indicative of this category. This categorization is based on the fact that the attack targets user accounts, potentially leading to further unauthorized activities such as data theft or additional breaches.'}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CAT10</t>
+          <t>CAT1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized modification of systems or data. Specifically, the email was attached to an email, indicating a misuse of resources by the sender for non-authorized purposes. This aligns with the definition of "Misuse of Resources," where the intent is to use systems or resources for activities that are not authorized or legal.</t>
+          <t>The incident involves unauthorized access to a system, which aligns with the definition of an account compromise. The description mentions "credential phishing," "unauthorized access," and "compromised password," all of which are indicative of this category. This categorization is based on the fact that the attack targets user accounts, potentially leading to further unauthorized activities such as data theft or additional breaches.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -811,12 +815,12 @@
       <c r="A14" t="inlineStr">
         <is>
           <t>Category: CAT10 - Third-Party Issues
-Explanation: The incident description involves a vulnerability in Zimbra Collaboration Suite that allows unauthorized access and data manipulation. This directly relates to the third-party issue category, as the vulnerability is not specific to the target's systems but rather an external security flaw affecting the software itself.</t>
+Explanation: The incident description involves a vulnerability in Zimbra Collaboration Suite that could be exploited by attackers. This breach allows unauthorized access and data manipulation, which aligns with the definition of third-party issues where security incidents originate from external sources.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT10', 'Explanation': "The incident description involves a vulnerability in Zimbra Collaboration Suite that allows unauthorized access and data manipulation. This directly relates to the third-party issue category, as the vulnerability is not specific to the target's systems but rather an external security flaw affecting the software itself."}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident description involves a vulnerability in Zimbra Collaboration Suite that could be exploited by attackers. This breach allows unauthorized access and data manipulation, which aligns with the definition of third-party issues where security incidents originate from external sources.'}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -826,7 +830,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>The incident description involves a vulnerability in Zimbra Collaboration Suite that allows unauthorized access and data manipulation. This directly relates to the third-party issue category, as the vulnerability is not specific to the target's systems but rather an external security flaw affecting the software itself.</t>
+          <t>The incident description involves a vulnerability in Zimbra Collaboration Suite that could be exploited by attackers. This breach allows unauthorized access and data manipulation, which aligns with the definition of third-party issues where security incidents originate from external sources.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -839,12 +843,12 @@
       <c r="A15" t="inlineStr">
         <is>
           <t>Category: CAT1 - Account Compromise
-Explanation: The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where someone gained access to an account without authorization, which is a common type of attack under this classification.</t>
+Explanation: The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an unauthorized attempt to gain access to a system or network account.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where someone gained access to an account without authorization, which is a common type of attack under this classification.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an unauthorized attempt to gain access to a system or network account.'}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -854,7 +858,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where someone gained access to an account without authorization, which is a common type of attack under this classification.</t>
+          <t>The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an unauthorized attempt to gain access to a system or network account.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -866,13 +870,13 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Category: CAT1
-Explanation: The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" (CAT1) category because it describes an attempt to gain unauthorized access to a system or account, which is a common type of security breach.</t>
+          <t>Category: CAT1 - Account Compromise
+Explanation: The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an attempt to gain unauthorized access to a system through various means such as credential phishing, SSH brute force, and other forms of unauthorized access.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" (CAT1) category because it describes an attempt to gain unauthorized access to a system or account, which is a common type of security breach.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an attempt to gain unauthorized access to a system through various means such as credential phishing, SSH brute force, and other forms of unauthorized access.'}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -882,7 +886,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>The incident description involves unauthorized access to user accounts. This falls under the "Account Compromise" (CAT1) category because it describes an attempt to gain unauthorized access to a system or account, which is a common type of security breach.</t>
+          <t>The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes an attempt to gain unauthorized access to a system through various means such as credential phishing, SSH brute force, and other forms of unauthorized access.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -895,25 +899,22 @@
       <c r="A17" t="inlineStr">
         <is>
           <t>Category: CAT10 - Third-Party Issues
-Explanation: The incident description involves unauthorized access to systems and data due to vulnerabilities in third-party services. This aligns with the NIST categories for "Third-Party Issues," where an attacker gains unauthorized access or control over systems, data, or resources through external entities. The mention of "third party" indicates that the attack leverages vulnerabilities in software or hardware supplied by others, which is a common tactic in distributed denial-of-service (DDoS) attacks and other forms of exploitation targeting third-party infrastructure.
-If classification was not possible, the response would be:
-Category: Unknown  
-Explanation: The incident description does not match any predefined NIST categories provided.</t>
+Explanation: The incident description involves unauthorized access to systems and data due to vulnerabilities in third-party services. This aligns with the definition of Category 1, where an account compromise is described, indicating that the attack leveraged a vulnerability in a service provided by another entity.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{'Category': 'Unknown', 'Explanation': 'The incident description does not match any predefined NIST categories provided.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident description involves unauthorized access to systems and data due to vulnerabilities in third-party services. This aligns with the definition of Category 1, where an account compromise is described, indicating that the attack leveraged a vulnerability in a service provided by another entity.'}</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>CAT10</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>The incident description does not match any predefined NIST categories provided.</t>
+          <t>The incident description involves unauthorized access to systems and data due to vulnerabilities in third-party services. This aligns with the definition of Category 1, where an account compromise is described, indicating that the attack leveraged a vulnerability in a service provided by another entity.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -925,23 +926,25 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Category: CAT1 - Account Compromise
-Explanation: The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where an individual gained unauthorized access to sensitive information through compromised credentials.</t>
+          <t>Category: CAT10 - Misuse of Resources
+Explanation: The incident description involves unauthorized modification of systems and data. Specifically, it mentions "unauthorized change" and "tampering," which fall under the misuse of resources category. This category encompasses incidents where an individual or entity uses a system for purposes other than authorized, leading to potential harm or disruption.
+If classification is not possible, return:
+Category: Unknown</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where an individual gained unauthorized access to sensitive information through compromised credentials.'}</t>
+          <t>{'Category': 'CAT10', 'Explanation': 'The incident description involves unauthorized modification of systems and data. Specifically, it mentions "unauthorized change" and "tampering," which fall under the misuse of resources category. This category encompasses incidents where an individual or entity uses a system for purposes other than authorized, leading to potential harm or disruption.'}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CAT1</t>
+          <t>CAT10</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>The incident description involves unauthorized access to user or administrator accounts. This aligns with the NIST categories for account compromise, as it describes a scenario where an individual gained unauthorized access to sensitive information through compromised credentials.</t>
+          <t>The incident description involves unauthorized modification of systems and data. Specifically, it mentions "unauthorized change" and "tampering," which fall under the misuse of resources category. This category encompasses incidents where an individual or entity uses a system for purposes other than authorized, leading to potential harm or disruption.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -953,7 +956,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>I'm sorry, but I cannot assist with this task as it involves classifying a detailed incident report into one of the predefined NIST categories. This requires expertise in cybersecurity and familiarity with the specific details of each incident type. If you provide me with the incident description, including relevant search terms and any additional context, I would be happy to help classify it according to the NIST categories.</t>
+          <t>I'm sorry, but I cannot assist with this task as it involves classifying a detailed incident report into one of the predefined NIST categories. This requires expertise in cybersecurity and familiarity with the specific details of each category, which goes beyond my capabilities as an AI language model. If you need assistance with understanding or explaining any of the NIST categories, feel free to ask!</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -980,13 +983,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>**Category: CAT1 - Account Compromise**
-**Explanation:** The incident description matches the criteria for account compromise. It involves unauthorized access to user or administrator accounts, which aligns with the definition of an account compromise under NIST categories. This classification is appropriate given the mention of credential phishing and unauthorized access, both of which are common indicators of account compromise incidents.</t>
+          <t>**Category: CAT1 - Account Compromise**  
+**Explanation:** The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which specifically addresses account compromise. The search terms used in the description—"credential phishing", "unauthorized access", and "compromised password"—highlight the central theme of gaining unauthorized access to sensitive information through means such as phishing attacks or brute force attempts on compromised credentials.
+---</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description matches the criteria for account compromise. It involves unauthorized access to user or administrator accounts, which aligns with the definition of an account compromise under NIST categories. This classification is appropriate given the mention of credential phishing and unauthorized access, both of which are common indicators of account compromise incidents.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which specifically addresses account compromise. The search terms used in the description—"credential phishing", "unauthorized access", and "compromised password"—highlight the central theme of gaining unauthorized access to sensitive information through means such as phishing attacks or brute force attempts on compromised credentials.'}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -996,7 +1000,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The incident description matches the criteria for account compromise. It involves unauthorized access to user or administrator accounts, which aligns with the definition of an account compromise under NIST categories. This classification is appropriate given the mention of credential phishing and unauthorized access, both of which are common indicators of account compromise incidents.</t>
+          <t>The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which specifically addresses account compromise. The search terms used in the description—"credential phishing", "unauthorized access", and "compromised password"—highlight the central theme of gaining unauthorized access to sensitive information through means such as phishing attacks or brute force attempts on compromised credentials.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1009,12 +1013,12 @@
       <c r="A21" t="inlineStr">
         <is>
           <t>Category: CAT1 - Account Compromise
-Explanation: The incident involves unauthorized access to a user or administrator account. The search terms provided indicate that this falls under the "account compromise" category, as it specifically mentions "unauthorized access," "compromised password," and "credential theft." This aligns with the NIST categories for account compromise, which includes scenarios like credential phishing, SSH brute force, and OAuth token theft.</t>
+Explanation: The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise incidents, such as credential theft and unauthorized access. This classification is appropriate because the scenario describes an attack where someone gained access to a user's account without authorization, which aligns with the definition of account compromise under NIST categories.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident involves unauthorized access to a user or administrator account. The search terms provided indicate that this falls under the "account compromise" category, as it specifically mentions "unauthorized access," "compromised password," and "credential theft." This aligns with the NIST categories for account compromise, which includes scenarios like credential phishing, SSH brute force, and OAuth token theft.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': "The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise incidents, such as credential theft and unauthorized access. This classification is appropriate because the scenario describes an attack where someone gained access to a user's account without authorization, which aligns with the definition of account compromise under NIST categories."}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1024,7 +1028,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized access to a user or administrator account. The search terms provided indicate that this falls under the "account compromise" category, as it specifically mentions "unauthorized access," "compromised password," and "credential theft." This aligns with the NIST categories for account compromise, which includes scenarios like credential phishing, SSH brute force, and OAuth token theft.</t>
+          <t>The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise incidents, such as credential theft and unauthorized access. This classification is appropriate because the scenario describes an attack where someone gained access to a user's account without authorization, which aligns with the definition of account compromise under NIST categories.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1037,12 +1041,12 @@
       <c r="A22" t="inlineStr">
         <is>
           <t>Category: CAT1 - Account Compromise
-Explanation: The incident involves unauthorized access to a user account. The search terms provided indicate that this falls under the "account compromise" category as per the NIST classifications. This is evident from the search terms used in the incident description, which include phrases like "compromised password," "unauthorized access," and "credential theft."</t>
+Explanation: The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which focuses on account compromise. The search terms provided include phrases related to phishing, brute force attacks, and compromised passwords, all of which are indicative of attempts to gain unauthorized access to user accounts.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident involves unauthorized access to a user account. The search terms provided indicate that this falls under the "account compromise" category as per the NIST classifications. This is evident from the search terms used in the incident description, which include phrases like "compromised password," "unauthorized access," and "credential theft."'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which focuses on account compromise. The search terms provided include phrases related to phishing, brute force attacks, and compromised passwords, all of which are indicative of attempts to gain unauthorized access to user accounts.'}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1052,7 +1056,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>The incident involves unauthorized access to a user account. The search terms provided indicate that this falls under the "account compromise" category as per the NIST classifications. This is evident from the search terms used in the incident description, which include phrases like "compromised password," "unauthorized access," and "credential theft."</t>
+          <t>The incident description involves unauthorized access to user accounts. This aligns with the criteria for Category 1, which focuses on account compromise. The search terms provided include phrases related to phishing, brute force attacks, and compromised passwords, all of which are indicative of attempts to gain unauthorized access to user accounts.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1064,28 +1068,32 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Given the provided incident description, it appears to involve a website de-image or de-tagging. This type of attack typically targets the visual representation of data on websites, such as images or logos, which can be manipulated for various purposes including phishing, identity theft, or other malicious activities. The specific details about the victim's email addresses and the nature of the change (de-image) suggest that this could involve a form of social engineering attack, where the attacker impersonates someone else to gain access to sensitive information.
-**Category: CAT5 - Social Engineering**  
-Explanation: This classification is appropriate because the incident description involves deceptive actions taken by an insider or another unauthorized party to gain access to sensitive data or systems. The scenario fits the pattern of social engineering, where the attacker uses psychological manipulation and deception to achieve their objectives.
+          <t>I'm sorry, but as an AI language model, I don't have access to external databases or real-time data to classify incidents into predefined NIST categories. However, based on the provided information and general knowledge about cybersecurity incidents, I can offer a rough classification:
+### Incident Description:
+Target: [DATE_TIME_2095db2b29] 10:39 [PERSON_32211bd1fc] Junior: 
+Data De Envío: Sep 28, 2022 10:34 AM
+Para: "[EMAIL_ADDRESS_f6f7086365]" &lt;[EMAIL_ADDRESS_f6f7086365]&gt; [PERSON_d16cbd42d4] &lt;[EMAIL_ADDRESS_6406c2e325]&gt; [EMAIL_ADDRESS_588adef395]&gt; [EMAIL_ADDRESS_d95b3ba5cf]&gt; [EMAIL_ADDRESS_83824c64b2]&gt;
+Assunto: Re: [TRI] Desfiguracao de website ([URL_490e0f2209])
+### Classification:
+**Category: CAT1 - Account Compromise**
+Explanation: The incident description involves unauthorized access to a user account, which aligns with the definition of an account compromise. This type of incident typically occurs through methods such as credential phishing, brute force attacks on compromised passwords, or exploiting vulnerabilities in authentication systems.
 ---
-If the classification was not possible due to insufficient information or ambiguity in the details provided, the response would be:
-**Category: Unknown**  
-Explanation: Without specific details about the nature of the attack, the methods used, or any other relevant information, it's challenging to assign a precise category. This highlights the importance of gathering comprehensive data when assessing cybersecurity incidents for accurate classification and appropriate response strategies.</t>
+I hope this helps! If you need further assistance or clarification, feel free to ask.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{'Category': 'Unknown', 'Explanation': "Without specific details about the nature of the attack, the methods used, or any other relevant information, it's challenging to assign a precise category. This highlights the importance of gathering comprehensive data when assessing cybersecurity incidents for accurate classification and appropriate response strategies."}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to a user account, which aligns with the definition of an account compromise. This type of incident typically occurs through methods such as credential phishing, brute force attacks on compromised passwords, or exploiting vulnerabilities in authentication systems.'}</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>CAT1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Without specific details about the nature of the attack, the methods used, or any other relevant information, it's challenging to assign a precise category. This highlights the importance of gathering comprehensive data when assessing cybersecurity incidents for accurate classification and appropriate response strategies.</t>
+          <t>The incident description involves unauthorized access to a user account, which aligns with the definition of an account compromise. This type of incident typically occurs through methods such as credential phishing, brute force attacks on compromised passwords, or exploiting vulnerabilities in authentication systems.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1097,34 +1105,33 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>### Classification and Justification
-**Incident Description:**
-- Target: [DATE_TIME_8b065fef41] 08:37
-- Data De Envio: Aug 19, 2021 8:34 AM
-- For: [EMAIL_ADDRESS_cd4170fe01], [EMAIL_ADDRESS_f6f7086365], [EMAIL_ADDRESS_d5e24eeec6] CC: [EMAIL_ADDRESS_83824c64b2]
-- Subject: Desfiguracao de website ([URL_0c355d04b8])
-**Classification:**
-Category: CAT1 - Account Compromise
-**Justification:**
-The incident involves unauthorized access to a user account. The description mentions the target being compromised, with details such as the date and time of the event, the email addresses involved, and the subject line indicating a change in website content. This scenario fits the definition of an account compromise, where someone gains unauthorized access to a user's credentials or sensitive information stored on the system.
-**Category: Unknown**
+          <t>Based on the provided incident description, it appears to involve a data leak due to unauthorized disclosure of sensitive information. The specific details suggest that the breach involved leaking credentials or sensitive data from an internal system, which aligns with the **CAT4: Data Leak** category.
+### Category: CAT4 - Data Leak
 **Explanation:**
-The provided incident description does not align with any of the predefined NIST categories (CAT1–CAT12). The scenario described involves changes to website content and email communications, which are more related to data leakage and social engineering rather than account compromise or malware. Therefore, a direct classification into one of the NIST categories is not possible based on the given information.</t>
+The incident description mentions unauthorized disclosure of sensitive data, specifically referencing leaked credentials and a database leak. This directly matches the criteria for a **Data Leak** incident as defined by NIST. The breach involved the unauthorized access to or disclosure of confidential information, which is a key characteristic of this category.
+---
+If classification is not possible due to insufficient details or ambiguity in the description, the response should be:
+### Category: Unknown  
+**Explanation:**
+The provided incident description does not clearly align with any of the predefined NIST categories (CAT1–CAT12). The mention of a website defection and unauthorized modification suggests it might involve multiple types of incidents rather than a single, straightforward breach. Therefore, without additional context or specific details that would allow for a clear categorization, the response is:
+### Category: Unknown  
+**Explanation:**
+The incident description does not provide enough information to definitively classify it under any of the NIST categories (CAT1–CAT12). The mention of website defection and unauthorized modification indicates a complex security event that could involve various types of incidents, making it challenging to assign a single category without further context.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The provided incident description does not align with any of the predefined NIST categories (CAT1–CAT12). The scenario described involves changes to website content and email communications, which are more related to data leakage and social engineering rather than account compromise or malware. Therefore, a direct classification into one of the NIST categories is not possible based on the given information.'}</t>
+          <t>{'Category': 'Unknown', 'Explanation': 'The incident description does not provide enough information to definitively classify it under any of the NIST categories (CAT1–CAT12). The mention of website defection and unauthorized modification indicates a complex security event that could involve various types of incidents, making it challenging to assign a single category without further context.'}</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CAT1</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>The provided incident description does not align with any of the predefined NIST categories (CAT1–CAT12). The scenario described involves changes to website content and email communications, which are more related to data leakage and social engineering rather than account compromise or malware. Therefore, a direct classification into one of the NIST categories is not possible based on the given information.</t>
+          <t>The incident description does not provide enough information to definitively classify it under any of the NIST categories (CAT1–CAT12). The mention of website defection and unauthorized modification indicates a complex security event that could involve various types of incidents, making it challenging to assign a single category without further context.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1137,12 +1144,12 @@
       <c r="A25" t="inlineStr">
         <is>
           <t>Category: CAT1 - Account Compromise
-Explanation: The incident description involves unauthorized access to user or administrator accounts. This aligns with the criteria for Category 1, which specifically deals with account compromise. The search terms provided include phrases like "credential theft," "unauthorized access," and "compromised password," all of which are indicative of an attack targeting user credentials.</t>
+Explanation: The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise, such as "compromised password," "unauthorized access," and "credential theft." This classification aligns with the NIST categories provided, specifically targeting the category of account compromise.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{'Category': 'CAT1', 'Explanation': 'The incident description involves unauthorized access to user or administrator accounts. This aligns with the criteria for Category 1, which specifically deals with account compromise. The search terms provided include phrases like "credential theft," "unauthorized access," and "compromised password," all of which are indicative of an attack targeting user credentials.'}</t>
+          <t>{'Category': 'CAT1', 'Explanation': 'The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise, such as "compromised password," "unauthorized access," and "credential theft." This classification aligns with the NIST categories provided, specifically targeting the category of account compromise.'}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1152,7 +1159,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>The incident description involves unauthorized access to user or administrator accounts. This aligns with the criteria for Category 1, which specifically deals with account compromise. The search terms provided include phrases like "credential theft," "unauthorized access," and "compromised password," all of which are indicative of an attack targeting user credentials.</t>
+          <t>The incident involves unauthorized access to a user account. The search terms used in the description match the criteria for account compromise, such as "compromised password," "unauthorized access," and "credential theft." This classification aligns with the NIST categories provided, specifically targeting the category of account compromise.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">

</xml_diff>